<commit_message>
corrigido catch rate de alguns pokemon que estavam com catch rate zerado
</commit_message>
<xml_diff>
--- a/pokemonv2/info/pokemons.xlsx
+++ b/pokemonv2/info/pokemons.xlsx
@@ -8734,8 +8734,8 @@
   <dimension ref="A1:H1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A702" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B711" sqref="B711"/>
+      <pane ySplit="1" topLeftCell="A688" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L691" sqref="L691"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>